<commit_message>
Modification du journal de bord
</commit_message>
<xml_diff>
--- a/Journée d'activité/Joshua.xlsx
+++ b/Journée d'activité/Joshua.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3FE36714-9E7B-4B2E-A0E1-2FC1334ECF06}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E764861-516C-4638-9F5C-CDFBA329A8B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3" uniqueCount="3">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>DATE</t>
   </si>
@@ -29,6 +29,9 @@
   </si>
   <si>
     <t>Création du GitHub / Journal d'activité / reglage problème gitHub</t>
+  </si>
+  <si>
+    <t>Choix du template/Réalisation de la page thème</t>
   </si>
 </sst>
 </file>
@@ -200,6 +203,33 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -208,33 +238,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -519,7 +522,7 @@
   <dimension ref="B2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:H11"/>
+      <selection activeCell="C6" sqref="C6:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -532,291 +535,318 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>43756</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="13"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
+      <c r="B6" s="10">
+        <v>43777</v>
+      </c>
+      <c r="C6" s="4" t="s">
+        <v>3</v>
+      </c>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
+      <c r="B8" s="2"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="10"/>
+      <c r="B9" s="3"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="13"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="12"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="10"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="7"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="7"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="13"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="7"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="10"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="7"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="6"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="10"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="7"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="13"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="7"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="12"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="10"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="7"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="6"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="12"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="10"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="13"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="7"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="12"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="10"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="31">
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C22:H23"/>
+    <mergeCell ref="C26:H27"/>
+    <mergeCell ref="C28:H29"/>
+    <mergeCell ref="C30:H31"/>
+    <mergeCell ref="C32:H33"/>
+    <mergeCell ref="C24:H25"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="C4:H5"/>
+    <mergeCell ref="C16:H17"/>
+    <mergeCell ref="C18:H19"/>
+    <mergeCell ref="C20:H21"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="C6:H7"/>
+    <mergeCell ref="C8:H9"/>
+    <mergeCell ref="C10:H11"/>
+    <mergeCell ref="C12:H13"/>
+    <mergeCell ref="C14:H15"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
     <mergeCell ref="B30:B31"/>
     <mergeCell ref="B32:B33"/>
     <mergeCell ref="B18:B19"/>
@@ -825,29 +855,6 @@
     <mergeCell ref="B24:B25"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B16:B17"/>
-    <mergeCell ref="C6:H7"/>
-    <mergeCell ref="C8:H9"/>
-    <mergeCell ref="C10:H11"/>
-    <mergeCell ref="C12:H13"/>
-    <mergeCell ref="C14:H15"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="C4:H5"/>
-    <mergeCell ref="C16:H17"/>
-    <mergeCell ref="C18:H19"/>
-    <mergeCell ref="C20:H21"/>
-    <mergeCell ref="C22:H23"/>
-    <mergeCell ref="C26:H27"/>
-    <mergeCell ref="C28:H29"/>
-    <mergeCell ref="C30:H31"/>
-    <mergeCell ref="C32:H33"/>
-    <mergeCell ref="C24:H25"/>
-    <mergeCell ref="C3:H3"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ajout du fichier pour Paul et Modification des fichiers journée d'activités
</commit_message>
<xml_diff>
--- a/Journée d'activité/Joshua.xlsx
+++ b/Journée d'activité/Joshua.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E764861-516C-4638-9F5C-CDFBA329A8B7}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9F1AB5-0601-4D2B-9F2A-1C758FD447F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -31,7 +31,7 @@
     <t>Création du GitHub / Journal d'activité / reglage problème gitHub</t>
   </si>
   <si>
-    <t>Choix du template/Réalisation de la page thème</t>
+    <t>Choix du template/ Prise en main du template/ Test d'ajout d'un fichier .mp3 en HTML</t>
   </si>
 </sst>
 </file>
@@ -203,41 +203,41 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -521,8 +521,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:H33"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C6" sqref="C6:H7"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="J14" sqref="J14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,300 +535,305 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="10">
+      <c r="B4" s="11">
         <v>43756</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="10">
+      <c r="B6" s="11">
         <v>43777</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="2"/>
-      <c r="C8" s="4"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
+      <c r="B8" s="13"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="3"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
+      <c r="B9" s="12"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
+      <c r="B10" s="13"/>
+      <c r="C10" s="5"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="10"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="6"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="9"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="9"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="6"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="9"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="10"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="6"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="9"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="10"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="6"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="9"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="6"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="7"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="9"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="10"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="6"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="9"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="6"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="7"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="9"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C22:H23"/>
-    <mergeCell ref="C26:H27"/>
-    <mergeCell ref="C28:H29"/>
-    <mergeCell ref="C30:H31"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
     <mergeCell ref="C32:H33"/>
     <mergeCell ref="C24:H25"/>
     <mergeCell ref="B4:B5"/>
@@ -845,16 +850,11 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C22:H23"/>
+    <mergeCell ref="C26:H27"/>
+    <mergeCell ref="C28:H29"/>
+    <mergeCell ref="C30:H31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Modification du journal d'activité
</commit_message>
<xml_diff>
--- a/Journée d'activité/Joshua.xlsx
+++ b/Journée d'activité/Joshua.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B9F1AB5-0601-4D2B-9F2A-1C758FD447F6}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5429A92B-F64E-496E-850A-268B7CC251A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>DATE</t>
   </si>
@@ -32,6 +32,9 @@
   </si>
   <si>
     <t>Choix du template/ Prise en main du template/ Test d'ajout d'un fichier .mp3 en HTML</t>
+  </si>
+  <si>
+    <t>Discussion autour du design du site ainsi que sur les différentes classes de la BDD/Création login.php + theme.html</t>
   </si>
 </sst>
 </file>
@@ -198,11 +201,38 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -212,31 +242,7 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -522,7 +528,7 @@
   <dimension ref="B2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J14" sqref="J14"/>
+      <selection activeCell="J8" sqref="J8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -535,305 +541,304 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="11" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
+      <c r="D3" s="12"/>
+      <c r="E3" s="12"/>
+      <c r="F3" s="12"/>
+      <c r="G3" s="12"/>
+      <c r="H3" s="13"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>43756</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>43777</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="13"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
-    </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B9" s="12"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="10"/>
+      <c r="B8" s="10">
+        <v>43784</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
+    </row>
+    <row r="9" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B9" s="14"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="13"/>
-      <c r="C10" s="5"/>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
+      <c r="B10" s="2"/>
+      <c r="C10" s="4"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="13"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="12"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="10"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="7"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="7"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="13"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="7"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="10"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="7"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="6"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="10"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="7"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="13"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="7"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="12"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="10"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="7"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="6"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="12"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="10"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="13"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="7"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="12"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="10"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C22:H23"/>
+    <mergeCell ref="C26:H27"/>
+    <mergeCell ref="C28:H29"/>
+    <mergeCell ref="C30:H31"/>
     <mergeCell ref="C32:H33"/>
     <mergeCell ref="C24:H25"/>
     <mergeCell ref="B4:B5"/>
@@ -850,11 +855,16 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C22:H23"/>
-    <mergeCell ref="C26:H27"/>
-    <mergeCell ref="C28:H29"/>
-    <mergeCell ref="C30:H31"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Prédiction d'activité du jour dans le journal d'activité
</commit_message>
<xml_diff>
--- a/Journée d'activité/Joshua.xlsx
+++ b/Journée d'activité/Joshua.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5429A92B-F64E-496E-850A-268B7CC251A0}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB392E68-5054-4260-BF45-8B0623D1ACA2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
     <t>DATE</t>
   </si>
@@ -35,6 +35,9 @@
   </si>
   <si>
     <t>Discussion autour du design du site ainsi que sur les différentes classes de la BDD/Création login.php + theme.html</t>
+  </si>
+  <si>
+    <t>Travail sur login.php et mise en commun afin d'évaluer les tâches restantes (prédictions)</t>
   </si>
 </sst>
 </file>
@@ -206,33 +209,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -241,6 +217,33 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -528,7 +531,7 @@
   <dimension ref="B2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="J8" sqref="J8"/>
+      <selection activeCell="C10" sqref="C10:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -541,304 +544,313 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="11" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="12"/>
-      <c r="E3" s="12"/>
-      <c r="F3" s="12"/>
-      <c r="G3" s="12"/>
-      <c r="H3" s="13"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="10">
+      <c r="B4" s="11">
         <v>43756</v>
       </c>
-      <c r="C4" s="4" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-      <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="7"/>
-      <c r="D5" s="8"/>
-      <c r="E5" s="8"/>
-      <c r="F5" s="8"/>
-      <c r="G5" s="8"/>
-      <c r="H5" s="9"/>
+      <c r="B5" s="12"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="10">
+      <c r="B6" s="11">
         <v>43777</v>
       </c>
-      <c r="C6" s="4" t="s">
+      <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-      <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="7"/>
-      <c r="D7" s="8"/>
-      <c r="E7" s="8"/>
-      <c r="F7" s="8"/>
-      <c r="G7" s="8"/>
-      <c r="H7" s="9"/>
+      <c r="B7" s="12"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="10">
+      <c r="B8" s="11">
         <v>43784</v>
       </c>
-      <c r="C8" s="4" t="s">
+      <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-      <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="14"/>
-      <c r="C9" s="7"/>
-      <c r="D9" s="8"/>
-      <c r="E9" s="8"/>
-      <c r="F9" s="8"/>
-      <c r="G9" s="8"/>
-      <c r="H9" s="9"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="2"/>
-      <c r="C10" s="4"/>
-      <c r="D10" s="5"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-      <c r="G10" s="5"/>
-      <c r="H10" s="6"/>
+      <c r="B10" s="11">
+        <v>43791</v>
+      </c>
+      <c r="C10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="3"/>
-      <c r="C11" s="7"/>
-      <c r="D11" s="8"/>
-      <c r="E11" s="8"/>
-      <c r="F11" s="8"/>
-      <c r="G11" s="8"/>
-      <c r="H11" s="9"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="2"/>
-      <c r="C12" s="4"/>
-      <c r="D12" s="5"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-      <c r="G12" s="5"/>
-      <c r="H12" s="6"/>
+      <c r="B12" s="13"/>
+      <c r="C12" s="5"/>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="3"/>
-      <c r="C13" s="7"/>
-      <c r="D13" s="8"/>
-      <c r="E13" s="8"/>
-      <c r="F13" s="8"/>
-      <c r="G13" s="8"/>
-      <c r="H13" s="9"/>
+      <c r="B13" s="12"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="2"/>
-      <c r="C14" s="4"/>
-      <c r="D14" s="5"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-      <c r="G14" s="5"/>
-      <c r="H14" s="6"/>
+      <c r="B14" s="13"/>
+      <c r="C14" s="5"/>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="3"/>
-      <c r="C15" s="7"/>
-      <c r="D15" s="8"/>
-      <c r="E15" s="8"/>
-      <c r="F15" s="8"/>
-      <c r="G15" s="8"/>
-      <c r="H15" s="9"/>
+      <c r="B15" s="12"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="2"/>
-      <c r="C16" s="4"/>
-      <c r="D16" s="5"/>
-      <c r="E16" s="5"/>
-      <c r="F16" s="5"/>
-      <c r="G16" s="5"/>
-      <c r="H16" s="6"/>
+      <c r="B16" s="13"/>
+      <c r="C16" s="5"/>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="3"/>
-      <c r="C17" s="7"/>
-      <c r="D17" s="8"/>
-      <c r="E17" s="8"/>
-      <c r="F17" s="8"/>
-      <c r="G17" s="8"/>
-      <c r="H17" s="9"/>
+      <c r="B17" s="12"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="10"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="2"/>
-      <c r="C18" s="4"/>
-      <c r="D18" s="5"/>
-      <c r="E18" s="5"/>
-      <c r="F18" s="5"/>
-      <c r="G18" s="5"/>
-      <c r="H18" s="6"/>
+      <c r="B18" s="13"/>
+      <c r="C18" s="5"/>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="7"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="3"/>
-      <c r="C19" s="7"/>
-      <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
-      <c r="F19" s="8"/>
-      <c r="G19" s="8"/>
-      <c r="H19" s="9"/>
+      <c r="B19" s="12"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="10"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="4"/>
-      <c r="D20" s="5"/>
-      <c r="E20" s="5"/>
-      <c r="F20" s="5"/>
-      <c r="G20" s="5"/>
-      <c r="H20" s="6"/>
+      <c r="B20" s="13"/>
+      <c r="C20" s="5"/>
+      <c r="D20" s="6"/>
+      <c r="E20" s="6"/>
+      <c r="F20" s="6"/>
+      <c r="G20" s="6"/>
+      <c r="H20" s="7"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="7"/>
-      <c r="D21" s="8"/>
-      <c r="E21" s="8"/>
-      <c r="F21" s="8"/>
-      <c r="G21" s="8"/>
-      <c r="H21" s="9"/>
+      <c r="B21" s="12"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="4"/>
-      <c r="D22" s="5"/>
-      <c r="E22" s="5"/>
-      <c r="F22" s="5"/>
-      <c r="G22" s="5"/>
-      <c r="H22" s="6"/>
+      <c r="B22" s="13"/>
+      <c r="C22" s="5"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="7"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="7"/>
-      <c r="D23" s="8"/>
-      <c r="E23" s="8"/>
-      <c r="F23" s="8"/>
-      <c r="G23" s="8"/>
-      <c r="H23" s="9"/>
+      <c r="B23" s="12"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="10"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="5"/>
-      <c r="E24" s="5"/>
-      <c r="F24" s="5"/>
-      <c r="G24" s="5"/>
-      <c r="H24" s="6"/>
+      <c r="B24" s="13"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="7"/>
-      <c r="D25" s="8"/>
-      <c r="E25" s="8"/>
-      <c r="F25" s="8"/>
-      <c r="G25" s="8"/>
-      <c r="H25" s="9"/>
+      <c r="B25" s="12"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="10"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="5"/>
-      <c r="E26" s="5"/>
-      <c r="F26" s="5"/>
-      <c r="G26" s="5"/>
-      <c r="H26" s="6"/>
+      <c r="B26" s="13"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="7"/>
-      <c r="D27" s="8"/>
-      <c r="E27" s="8"/>
-      <c r="F27" s="8"/>
-      <c r="G27" s="8"/>
-      <c r="H27" s="9"/>
+      <c r="B27" s="12"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="4"/>
-      <c r="D28" s="5"/>
-      <c r="E28" s="5"/>
-      <c r="F28" s="5"/>
-      <c r="G28" s="5"/>
-      <c r="H28" s="6"/>
+      <c r="B28" s="13"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="7"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-      <c r="C29" s="7"/>
-      <c r="D29" s="8"/>
-      <c r="E29" s="8"/>
-      <c r="F29" s="8"/>
-      <c r="G29" s="8"/>
-      <c r="H29" s="9"/>
+      <c r="B29" s="12"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="10"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="4"/>
-      <c r="D30" s="5"/>
-      <c r="E30" s="5"/>
-      <c r="F30" s="5"/>
-      <c r="G30" s="5"/>
-      <c r="H30" s="6"/>
+      <c r="B30" s="13"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="C31" s="7"/>
-      <c r="D31" s="8"/>
-      <c r="E31" s="8"/>
-      <c r="F31" s="8"/>
-      <c r="G31" s="8"/>
-      <c r="H31" s="9"/>
+      <c r="B31" s="12"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="4"/>
-      <c r="D32" s="5"/>
-      <c r="E32" s="5"/>
-      <c r="F32" s="5"/>
-      <c r="G32" s="5"/>
-      <c r="H32" s="6"/>
+      <c r="B32" s="13"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="7"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-      <c r="C33" s="7"/>
-      <c r="D33" s="8"/>
-      <c r="E33" s="8"/>
-      <c r="F33" s="8"/>
-      <c r="G33" s="8"/>
-      <c r="H33" s="9"/>
+      <c r="B33" s="12"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C22:H23"/>
-    <mergeCell ref="C26:H27"/>
-    <mergeCell ref="C28:H29"/>
-    <mergeCell ref="C30:H31"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
     <mergeCell ref="C32:H33"/>
     <mergeCell ref="C24:H25"/>
     <mergeCell ref="B4:B5"/>
@@ -855,16 +867,11 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C22:H23"/>
+    <mergeCell ref="C26:H27"/>
+    <mergeCell ref="C28:H29"/>
+    <mergeCell ref="C30:H31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Journal d'activité + mise en commun des pages terminées
</commit_message>
<xml_diff>
--- a/Journée d'activité/Joshua.xlsx
+++ b/Journée d'activité/Joshua.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB392E68-5054-4260-BF45-8B0623D1ACA2}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2FF2191-D3F3-4393-8701-E1797E8A98BF}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -37,7 +37,7 @@
     <t>Discussion autour du design du site ainsi que sur les différentes classes de la BDD/Création login.php + theme.html</t>
   </si>
   <si>
-    <t>Travail sur login.php et mise en commun afin d'évaluer les tâches restantes (prédictions)</t>
+    <t>Terminer et vérifier le fonctionnement de la page login.php et mise en commun afin d'évaluer les tâches restantes (prédiction)</t>
   </si>
 </sst>
 </file>
@@ -209,6 +209,36 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -217,36 +247,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -531,7 +531,7 @@
   <dimension ref="B2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10:H11"/>
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -544,313 +544,308 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="12" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="F3" s="3"/>
-      <c r="G3" s="3"/>
-      <c r="H3" s="4"/>
+      <c r="D3" s="13"/>
+      <c r="E3" s="13"/>
+      <c r="F3" s="13"/>
+      <c r="G3" s="13"/>
+      <c r="H3" s="14"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="11">
+      <c r="B4" s="10">
         <v>43756</v>
       </c>
-      <c r="C4" s="5" t="s">
+      <c r="C4" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6"/>
-      <c r="F4" s="6"/>
-      <c r="G4" s="6"/>
-      <c r="H4" s="7"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+      <c r="G4" s="5"/>
+      <c r="H4" s="6"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="12"/>
-      <c r="C5" s="8"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
-      <c r="G5" s="9"/>
-      <c r="H5" s="10"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="8"/>
+      <c r="E5" s="8"/>
+      <c r="F5" s="8"/>
+      <c r="G5" s="8"/>
+      <c r="H5" s="9"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="11">
+      <c r="B6" s="10">
         <v>43777</v>
       </c>
-      <c r="C6" s="5" t="s">
+      <c r="C6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="6"/>
-      <c r="E6" s="6"/>
-      <c r="F6" s="6"/>
-      <c r="G6" s="6"/>
-      <c r="H6" s="7"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+      <c r="G6" s="5"/>
+      <c r="H6" s="6"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="12"/>
-      <c r="C7" s="8"/>
-      <c r="D7" s="9"/>
-      <c r="E7" s="9"/>
-      <c r="F7" s="9"/>
-      <c r="G7" s="9"/>
-      <c r="H7" s="10"/>
+      <c r="B7" s="3"/>
+      <c r="C7" s="7"/>
+      <c r="D7" s="8"/>
+      <c r="E7" s="8"/>
+      <c r="F7" s="8"/>
+      <c r="G7" s="8"/>
+      <c r="H7" s="9"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="11">
+      <c r="B8" s="10">
         <v>43784</v>
       </c>
-      <c r="C8" s="5" t="s">
+      <c r="C8" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="6"/>
-      <c r="E8" s="6"/>
-      <c r="F8" s="6"/>
-      <c r="G8" s="6"/>
-      <c r="H8" s="7"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+      <c r="G8" s="5"/>
+      <c r="H8" s="6"/>
     </row>
     <row r="9" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="14"/>
-      <c r="C9" s="8"/>
-      <c r="D9" s="9"/>
-      <c r="E9" s="9"/>
-      <c r="F9" s="9"/>
-      <c r="G9" s="9"/>
-      <c r="H9" s="10"/>
+      <c r="B9" s="11"/>
+      <c r="C9" s="7"/>
+      <c r="D9" s="8"/>
+      <c r="E9" s="8"/>
+      <c r="F9" s="8"/>
+      <c r="G9" s="8"/>
+      <c r="H9" s="9"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="11">
+      <c r="B10" s="10">
         <v>43791</v>
       </c>
-      <c r="C10" s="5" t="s">
+      <c r="C10" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="6"/>
-      <c r="E10" s="6"/>
-      <c r="F10" s="6"/>
-      <c r="G10" s="6"/>
-      <c r="H10" s="7"/>
-    </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B11" s="12"/>
-      <c r="C11" s="8"/>
-      <c r="D11" s="9"/>
-      <c r="E11" s="9"/>
-      <c r="F11" s="9"/>
-      <c r="G11" s="9"/>
-      <c r="H11" s="10"/>
+      <c r="D10" s="5"/>
+      <c r="E10" s="5"/>
+      <c r="F10" s="5"/>
+      <c r="G10" s="5"/>
+      <c r="H10" s="6"/>
+    </row>
+    <row r="11" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B11" s="3"/>
+      <c r="C11" s="7"/>
+      <c r="D11" s="8"/>
+      <c r="E11" s="8"/>
+      <c r="F11" s="8"/>
+      <c r="G11" s="8"/>
+      <c r="H11" s="9"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="13"/>
-      <c r="C12" s="5"/>
-      <c r="D12" s="6"/>
-      <c r="E12" s="6"/>
-      <c r="F12" s="6"/>
-      <c r="G12" s="6"/>
-      <c r="H12" s="7"/>
+      <c r="B12" s="2"/>
+      <c r="C12" s="4"/>
+      <c r="D12" s="5"/>
+      <c r="E12" s="5"/>
+      <c r="F12" s="5"/>
+      <c r="G12" s="5"/>
+      <c r="H12" s="6"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="12"/>
-      <c r="C13" s="8"/>
-      <c r="D13" s="9"/>
-      <c r="E13" s="9"/>
-      <c r="F13" s="9"/>
-      <c r="G13" s="9"/>
-      <c r="H13" s="10"/>
+      <c r="B13" s="3"/>
+      <c r="C13" s="7"/>
+      <c r="D13" s="8"/>
+      <c r="E13" s="8"/>
+      <c r="F13" s="8"/>
+      <c r="G13" s="8"/>
+      <c r="H13" s="9"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="13"/>
-      <c r="C14" s="5"/>
-      <c r="D14" s="6"/>
-      <c r="E14" s="6"/>
-      <c r="F14" s="6"/>
-      <c r="G14" s="6"/>
-      <c r="H14" s="7"/>
+      <c r="B14" s="2"/>
+      <c r="C14" s="4"/>
+      <c r="D14" s="5"/>
+      <c r="E14" s="5"/>
+      <c r="F14" s="5"/>
+      <c r="G14" s="5"/>
+      <c r="H14" s="6"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="12"/>
-      <c r="C15" s="8"/>
-      <c r="D15" s="9"/>
-      <c r="E15" s="9"/>
-      <c r="F15" s="9"/>
-      <c r="G15" s="9"/>
-      <c r="H15" s="10"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="7"/>
+      <c r="D15" s="8"/>
+      <c r="E15" s="8"/>
+      <c r="F15" s="8"/>
+      <c r="G15" s="8"/>
+      <c r="H15" s="9"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B16" s="13"/>
-      <c r="C16" s="5"/>
-      <c r="D16" s="6"/>
-      <c r="E16" s="6"/>
-      <c r="F16" s="6"/>
-      <c r="G16" s="6"/>
-      <c r="H16" s="7"/>
+      <c r="B16" s="2"/>
+      <c r="C16" s="4"/>
+      <c r="D16" s="5"/>
+      <c r="E16" s="5"/>
+      <c r="F16" s="5"/>
+      <c r="G16" s="5"/>
+      <c r="H16" s="6"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="12"/>
-      <c r="C17" s="8"/>
-      <c r="D17" s="9"/>
-      <c r="E17" s="9"/>
-      <c r="F17" s="9"/>
-      <c r="G17" s="9"/>
-      <c r="H17" s="10"/>
+      <c r="B17" s="3"/>
+      <c r="C17" s="7"/>
+      <c r="D17" s="8"/>
+      <c r="E17" s="8"/>
+      <c r="F17" s="8"/>
+      <c r="G17" s="8"/>
+      <c r="H17" s="9"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B18" s="13"/>
-      <c r="C18" s="5"/>
-      <c r="D18" s="6"/>
-      <c r="E18" s="6"/>
-      <c r="F18" s="6"/>
-      <c r="G18" s="6"/>
-      <c r="H18" s="7"/>
+      <c r="B18" s="2"/>
+      <c r="C18" s="4"/>
+      <c r="D18" s="5"/>
+      <c r="E18" s="5"/>
+      <c r="F18" s="5"/>
+      <c r="G18" s="5"/>
+      <c r="H18" s="6"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="12"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="9"/>
-      <c r="E19" s="9"/>
-      <c r="F19" s="9"/>
-      <c r="G19" s="9"/>
-      <c r="H19" s="10"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="7"/>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+      <c r="F19" s="8"/>
+      <c r="G19" s="8"/>
+      <c r="H19" s="9"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="13"/>
-      <c r="C20" s="5"/>
-      <c r="D20" s="6"/>
-      <c r="E20" s="6"/>
-      <c r="F20" s="6"/>
-      <c r="G20" s="6"/>
-      <c r="H20" s="7"/>
+      <c r="B20" s="2"/>
+      <c r="C20" s="4"/>
+      <c r="D20" s="5"/>
+      <c r="E20" s="5"/>
+      <c r="F20" s="5"/>
+      <c r="G20" s="5"/>
+      <c r="H20" s="6"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="12"/>
-      <c r="C21" s="8"/>
-      <c r="D21" s="9"/>
-      <c r="E21" s="9"/>
-      <c r="F21" s="9"/>
-      <c r="G21" s="9"/>
-      <c r="H21" s="10"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="7"/>
+      <c r="D21" s="8"/>
+      <c r="E21" s="8"/>
+      <c r="F21" s="8"/>
+      <c r="G21" s="8"/>
+      <c r="H21" s="9"/>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="13"/>
-      <c r="C22" s="5"/>
-      <c r="D22" s="6"/>
-      <c r="E22" s="6"/>
-      <c r="F22" s="6"/>
-      <c r="G22" s="6"/>
-      <c r="H22" s="7"/>
+      <c r="B22" s="2"/>
+      <c r="C22" s="4"/>
+      <c r="D22" s="5"/>
+      <c r="E22" s="5"/>
+      <c r="F22" s="5"/>
+      <c r="G22" s="5"/>
+      <c r="H22" s="6"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="12"/>
-      <c r="C23" s="8"/>
-      <c r="D23" s="9"/>
-      <c r="E23" s="9"/>
-      <c r="F23" s="9"/>
-      <c r="G23" s="9"/>
-      <c r="H23" s="10"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="7"/>
+      <c r="D23" s="8"/>
+      <c r="E23" s="8"/>
+      <c r="F23" s="8"/>
+      <c r="G23" s="8"/>
+      <c r="H23" s="9"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="13"/>
-      <c r="C24" s="5"/>
-      <c r="D24" s="6"/>
-      <c r="E24" s="6"/>
-      <c r="F24" s="6"/>
-      <c r="G24" s="6"/>
-      <c r="H24" s="7"/>
+      <c r="B24" s="2"/>
+      <c r="C24" s="4"/>
+      <c r="D24" s="5"/>
+      <c r="E24" s="5"/>
+      <c r="F24" s="5"/>
+      <c r="G24" s="5"/>
+      <c r="H24" s="6"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="12"/>
-      <c r="C25" s="8"/>
-      <c r="D25" s="9"/>
-      <c r="E25" s="9"/>
-      <c r="F25" s="9"/>
-      <c r="G25" s="9"/>
-      <c r="H25" s="10"/>
+      <c r="B25" s="3"/>
+      <c r="C25" s="7"/>
+      <c r="D25" s="8"/>
+      <c r="E25" s="8"/>
+      <c r="F25" s="8"/>
+      <c r="G25" s="8"/>
+      <c r="H25" s="9"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="13"/>
-      <c r="C26" s="5"/>
-      <c r="D26" s="6"/>
-      <c r="E26" s="6"/>
-      <c r="F26" s="6"/>
-      <c r="G26" s="6"/>
-      <c r="H26" s="7"/>
+      <c r="B26" s="2"/>
+      <c r="C26" s="4"/>
+      <c r="D26" s="5"/>
+      <c r="E26" s="5"/>
+      <c r="F26" s="5"/>
+      <c r="G26" s="5"/>
+      <c r="H26" s="6"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="12"/>
-      <c r="C27" s="8"/>
-      <c r="D27" s="9"/>
-      <c r="E27" s="9"/>
-      <c r="F27" s="9"/>
-      <c r="G27" s="9"/>
-      <c r="H27" s="10"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="7"/>
+      <c r="D27" s="8"/>
+      <c r="E27" s="8"/>
+      <c r="F27" s="8"/>
+      <c r="G27" s="8"/>
+      <c r="H27" s="9"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="13"/>
-      <c r="C28" s="5"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
-      <c r="F28" s="6"/>
-      <c r="G28" s="6"/>
-      <c r="H28" s="7"/>
+      <c r="B28" s="2"/>
+      <c r="C28" s="4"/>
+      <c r="D28" s="5"/>
+      <c r="E28" s="5"/>
+      <c r="F28" s="5"/>
+      <c r="G28" s="5"/>
+      <c r="H28" s="6"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="12"/>
-      <c r="C29" s="8"/>
-      <c r="D29" s="9"/>
-      <c r="E29" s="9"/>
-      <c r="F29" s="9"/>
-      <c r="G29" s="9"/>
-      <c r="H29" s="10"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="7"/>
+      <c r="D29" s="8"/>
+      <c r="E29" s="8"/>
+      <c r="F29" s="8"/>
+      <c r="G29" s="8"/>
+      <c r="H29" s="9"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="13"/>
-      <c r="C30" s="5"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="6"/>
-      <c r="H30" s="7"/>
+      <c r="B30" s="2"/>
+      <c r="C30" s="4"/>
+      <c r="D30" s="5"/>
+      <c r="E30" s="5"/>
+      <c r="F30" s="5"/>
+      <c r="G30" s="5"/>
+      <c r="H30" s="6"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="12"/>
-      <c r="C31" s="8"/>
-      <c r="D31" s="9"/>
-      <c r="E31" s="9"/>
-      <c r="F31" s="9"/>
-      <c r="G31" s="9"/>
-      <c r="H31" s="10"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="7"/>
+      <c r="D31" s="8"/>
+      <c r="E31" s="8"/>
+      <c r="F31" s="8"/>
+      <c r="G31" s="8"/>
+      <c r="H31" s="9"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="13"/>
-      <c r="C32" s="5"/>
-      <c r="D32" s="6"/>
-      <c r="E32" s="6"/>
-      <c r="F32" s="6"/>
-      <c r="G32" s="6"/>
-      <c r="H32" s="7"/>
+      <c r="B32" s="2"/>
+      <c r="C32" s="4"/>
+      <c r="D32" s="5"/>
+      <c r="E32" s="5"/>
+      <c r="F32" s="5"/>
+      <c r="G32" s="5"/>
+      <c r="H32" s="6"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="12"/>
-      <c r="C33" s="8"/>
-      <c r="D33" s="9"/>
-      <c r="E33" s="9"/>
-      <c r="F33" s="9"/>
-      <c r="G33" s="9"/>
-      <c r="H33" s="10"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="7"/>
+      <c r="D33" s="8"/>
+      <c r="E33" s="8"/>
+      <c r="F33" s="8"/>
+      <c r="G33" s="8"/>
+      <c r="H33" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="31">
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="B14:B15"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B18:B19"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C22:H23"/>
+    <mergeCell ref="C26:H27"/>
+    <mergeCell ref="C28:H29"/>
+    <mergeCell ref="C30:H31"/>
     <mergeCell ref="C32:H33"/>
     <mergeCell ref="C24:H25"/>
     <mergeCell ref="B4:B5"/>
@@ -867,11 +862,16 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B10:B11"/>
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C22:H23"/>
-    <mergeCell ref="C26:H27"/>
-    <mergeCell ref="C28:H29"/>
-    <mergeCell ref="C30:H31"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Journal d'activité et end.php et Login.php
</commit_message>
<xml_diff>
--- a/Journée d'activité/Joshua.xlsx
+++ b/Journée d'activité/Joshua.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21601"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA85B2B1-7E15-451B-8057-96BFC8DDB176}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D2C17FB7-29BE-4AA5-87DE-D28031A98B5D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="25440" windowHeight="15390" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
   <si>
     <t>DATE</t>
   </si>
@@ -40,58 +40,26 @@
     <t>Si le nombre de point du login saisie est supérieur à 50, alors on envoie au serveur "C'est gagné" et la page end.php s'affiche.</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Récupérer le serveur et le lancer correctement : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="22"/>
-        <color rgb="FFFF0000"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>X</t>
-    </r>
+    <t>Récupérer le serveur avec le Client pour envoyer une information via sockets</t>
   </si>
   <si>
-    <r>
-      <t xml:space="preserve">Mise en commun avec le reste du groupe. : </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="22"/>
-        <color theme="9"/>
-        <rFont val="Calibri"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>V</t>
-    </r>
+    <t>Si le nombre de point du login saisie est supérieur à 50, alors on envoie au serveur "C'est gagné" via sockets et la page end.php s'affiche.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Récupérer le serveur et le lancer correctement </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Mise en commun avec le reste du groupe. </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color rgb="FFFF0000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="22"/>
-      <color theme="9"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -282,39 +250,6 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -324,6 +259,36 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="12" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="11" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -331,6 +296,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -616,7 +584,7 @@
   <dimension ref="B2:H33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="C12" sqref="C12:H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -629,318 +597,325 @@
       <c r="B3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="D3" s="14"/>
-      <c r="E3" s="14"/>
-      <c r="F3" s="14"/>
-      <c r="G3" s="14"/>
-      <c r="H3" s="15"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+      <c r="G3" s="3"/>
+      <c r="H3" s="4"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B4" s="4">
+      <c r="B4" s="11">
         <v>43756</v>
       </c>
-      <c r="C4" s="7" t="s">
+      <c r="C4" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="8"/>
-      <c r="E4" s="8"/>
-      <c r="F4" s="8"/>
-      <c r="G4" s="8"/>
-      <c r="H4" s="9"/>
+      <c r="D4" s="6"/>
+      <c r="E4" s="6"/>
+      <c r="F4" s="6"/>
+      <c r="G4" s="6"/>
+      <c r="H4" s="7"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B5" s="3"/>
-      <c r="C5" s="10"/>
-      <c r="D5" s="11"/>
-      <c r="E5" s="11"/>
-      <c r="F5" s="11"/>
-      <c r="G5" s="11"/>
-      <c r="H5" s="12"/>
+      <c r="B5" s="14"/>
+      <c r="C5" s="8"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
+      <c r="G5" s="9"/>
+      <c r="H5" s="10"/>
     </row>
     <row r="6" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B6" s="4">
+      <c r="B6" s="11">
         <v>43777</v>
       </c>
-      <c r="C6" s="7" t="s">
+      <c r="C6" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="8"/>
-      <c r="E6" s="8"/>
-      <c r="F6" s="8"/>
-      <c r="G6" s="8"/>
-      <c r="H6" s="9"/>
+      <c r="D6" s="6"/>
+      <c r="E6" s="6"/>
+      <c r="F6" s="6"/>
+      <c r="G6" s="6"/>
+      <c r="H6" s="7"/>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B7" s="3"/>
-      <c r="C7" s="10"/>
-      <c r="D7" s="11"/>
-      <c r="E7" s="11"/>
-      <c r="F7" s="11"/>
-      <c r="G7" s="11"/>
-      <c r="H7" s="12"/>
+      <c r="B7" s="14"/>
+      <c r="C7" s="8"/>
+      <c r="D7" s="9"/>
+      <c r="E7" s="9"/>
+      <c r="F7" s="9"/>
+      <c r="G7" s="9"/>
+      <c r="H7" s="10"/>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B8" s="4">
+      <c r="B8" s="11">
         <v>43784</v>
       </c>
-      <c r="C8" s="7" t="s">
+      <c r="C8" s="5" t="s">
         <v>4</v>
       </c>
-      <c r="D8" s="8"/>
-      <c r="E8" s="8"/>
-      <c r="F8" s="8"/>
-      <c r="G8" s="8"/>
-      <c r="H8" s="9"/>
+      <c r="D8" s="6"/>
+      <c r="E8" s="6"/>
+      <c r="F8" s="6"/>
+      <c r="G8" s="6"/>
+      <c r="H8" s="7"/>
     </row>
     <row r="9" spans="2:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B9" s="6"/>
-      <c r="C9" s="10"/>
-      <c r="D9" s="11"/>
-      <c r="E9" s="11"/>
-      <c r="F9" s="11"/>
-      <c r="G9" s="11"/>
-      <c r="H9" s="12"/>
+      <c r="B9" s="13"/>
+      <c r="C9" s="8"/>
+      <c r="D9" s="9"/>
+      <c r="E9" s="9"/>
+      <c r="F9" s="9"/>
+      <c r="G9" s="9"/>
+      <c r="H9" s="10"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B10" s="4">
+      <c r="B10" s="11">
         <v>43791</v>
       </c>
-      <c r="C10" s="7" t="s">
+      <c r="C10" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D10" s="8"/>
-      <c r="E10" s="8"/>
-      <c r="F10" s="8"/>
-      <c r="G10" s="8"/>
-      <c r="H10" s="9"/>
+      <c r="D10" s="6"/>
+      <c r="E10" s="6"/>
+      <c r="F10" s="6"/>
+      <c r="G10" s="6"/>
+      <c r="H10" s="7"/>
     </row>
     <row r="11" spans="2:8" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B11" s="5"/>
-      <c r="C11" s="10"/>
-      <c r="D11" s="11"/>
-      <c r="E11" s="11"/>
-      <c r="F11" s="11"/>
-      <c r="G11" s="11"/>
-      <c r="H11" s="12"/>
+      <c r="B11" s="12"/>
+      <c r="C11" s="8"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="9"/>
+      <c r="F11" s="9"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="10"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B12" s="5"/>
-      <c r="C12" s="7" t="s">
+      <c r="B12" s="12"/>
+      <c r="C12" s="5" t="s">
+        <v>9</v>
+      </c>
+      <c r="D12" s="6"/>
+      <c r="E12" s="6"/>
+      <c r="F12" s="6"/>
+      <c r="G12" s="6"/>
+      <c r="H12" s="7"/>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B13" s="12"/>
+      <c r="C13" s="8"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="9"/>
+      <c r="F13" s="9"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="10"/>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B14" s="12"/>
+      <c r="C14" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D14" s="6"/>
+      <c r="E14" s="6"/>
+      <c r="F14" s="6"/>
+      <c r="G14" s="6"/>
+      <c r="H14" s="7"/>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B15" s="13"/>
+      <c r="C15" s="8"/>
+      <c r="D15" s="9"/>
+      <c r="E15" s="9"/>
+      <c r="F15" s="9"/>
+      <c r="G15" s="9"/>
+      <c r="H15" s="10"/>
+    </row>
+    <row r="16" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B16" s="11">
+        <v>43798</v>
+      </c>
+      <c r="C16" s="5" t="s">
+        <v>8</v>
+      </c>
+      <c r="D16" s="6"/>
+      <c r="E16" s="6"/>
+      <c r="F16" s="6"/>
+      <c r="G16" s="6"/>
+      <c r="H16" s="7"/>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B17" s="12"/>
+      <c r="C17" s="8"/>
+      <c r="D17" s="9"/>
+      <c r="E17" s="9"/>
+      <c r="F17" s="9"/>
+      <c r="G17" s="9"/>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B18" s="12"/>
+      <c r="C18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="D18" s="6"/>
+      <c r="E18" s="6"/>
+      <c r="F18" s="6"/>
+      <c r="G18" s="6"/>
+      <c r="H18" s="7"/>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B19" s="13"/>
+      <c r="C19" s="8"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="9"/>
+      <c r="F19" s="9"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="10"/>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B20" s="11">
+        <v>43805</v>
+      </c>
+      <c r="C20" s="15" t="s">
+        <v>6</v>
+      </c>
+      <c r="D20" s="16"/>
+      <c r="E20" s="16"/>
+      <c r="F20" s="16"/>
+      <c r="G20" s="16"/>
+      <c r="H20" s="17"/>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B21" s="12"/>
+      <c r="C21" s="8"/>
+      <c r="D21" s="9"/>
+      <c r="E21" s="9"/>
+      <c r="F21" s="9"/>
+      <c r="G21" s="9"/>
+      <c r="H21" s="10"/>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B22" s="12"/>
+      <c r="C22" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="D12" s="8"/>
-      <c r="E12" s="8"/>
-      <c r="F12" s="8"/>
-      <c r="G12" s="8"/>
-      <c r="H12" s="9"/>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B13" s="5"/>
-      <c r="C13" s="10"/>
-      <c r="D13" s="11"/>
-      <c r="E13" s="11"/>
-      <c r="F13" s="11"/>
-      <c r="G13" s="11"/>
-      <c r="H13" s="12"/>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B14" s="5"/>
-      <c r="C14" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D14" s="8"/>
-      <c r="E14" s="8"/>
-      <c r="F14" s="8"/>
-      <c r="G14" s="8"/>
-      <c r="H14" s="9"/>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B15" s="6"/>
-      <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
-      <c r="E15" s="11"/>
-      <c r="F15" s="11"/>
-      <c r="G15" s="11"/>
-      <c r="H15" s="12"/>
-    </row>
-    <row r="16" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B16" s="4">
-        <v>43798</v>
-      </c>
-      <c r="C16" s="7" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="8"/>
-      <c r="E16" s="8"/>
-      <c r="F16" s="8"/>
-      <c r="G16" s="8"/>
-      <c r="H16" s="9"/>
-    </row>
-    <row r="17" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B17" s="5"/>
-      <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
-      <c r="E17" s="11"/>
-      <c r="F17" s="11"/>
-      <c r="G17" s="11"/>
-      <c r="H17" s="12"/>
-    </row>
-    <row r="18" spans="2:8" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B18" s="5"/>
-      <c r="C18" s="7" t="s">
-        <v>5</v>
-      </c>
-      <c r="D18" s="8"/>
-      <c r="E18" s="8"/>
-      <c r="F18" s="8"/>
-      <c r="G18" s="8"/>
-      <c r="H18" s="9"/>
-    </row>
-    <row r="19" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B19" s="6"/>
-      <c r="C19" s="10"/>
-      <c r="D19" s="11"/>
-      <c r="E19" s="11"/>
-      <c r="F19" s="11"/>
-      <c r="G19" s="11"/>
-      <c r="H19" s="12"/>
-    </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B20" s="2"/>
-      <c r="C20" s="16"/>
-      <c r="D20" s="17"/>
-      <c r="E20" s="17"/>
-      <c r="F20" s="17"/>
-      <c r="G20" s="17"/>
-      <c r="H20" s="18"/>
-    </row>
-    <row r="21" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B21" s="3"/>
-      <c r="C21" s="10"/>
-      <c r="D21" s="11"/>
-      <c r="E21" s="11"/>
-      <c r="F21" s="11"/>
-      <c r="G21" s="11"/>
-      <c r="H21" s="12"/>
-    </row>
-    <row r="22" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B22" s="2"/>
-      <c r="C22" s="7"/>
-      <c r="D22" s="8"/>
-      <c r="E22" s="8"/>
-      <c r="F22" s="8"/>
-      <c r="G22" s="8"/>
-      <c r="H22" s="9"/>
-    </row>
-    <row r="23" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B23" s="3"/>
-      <c r="C23" s="10"/>
-      <c r="D23" s="11"/>
-      <c r="E23" s="11"/>
-      <c r="F23" s="11"/>
-      <c r="G23" s="11"/>
-      <c r="H23" s="12"/>
+      <c r="D22" s="6"/>
+      <c r="E22" s="6"/>
+      <c r="F22" s="6"/>
+      <c r="G22" s="6"/>
+      <c r="H22" s="7"/>
+    </row>
+    <row r="23" spans="2:8" ht="36" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B23" s="13"/>
+      <c r="C23" s="8"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="9"/>
+      <c r="F23" s="9"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="10"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B24" s="2"/>
-      <c r="C24" s="7"/>
-      <c r="D24" s="8"/>
-      <c r="E24" s="8"/>
-      <c r="F24" s="8"/>
-      <c r="G24" s="8"/>
-      <c r="H24" s="9"/>
+      <c r="B24" s="18"/>
+      <c r="C24" s="5"/>
+      <c r="D24" s="6"/>
+      <c r="E24" s="6"/>
+      <c r="F24" s="6"/>
+      <c r="G24" s="6"/>
+      <c r="H24" s="7"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B25" s="3"/>
-      <c r="C25" s="10"/>
-      <c r="D25" s="11"/>
-      <c r="E25" s="11"/>
-      <c r="F25" s="11"/>
-      <c r="G25" s="11"/>
-      <c r="H25" s="12"/>
+      <c r="B25" s="14"/>
+      <c r="C25" s="8"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="9"/>
+      <c r="F25" s="9"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="10"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B26" s="2"/>
-      <c r="C26" s="7"/>
-      <c r="D26" s="8"/>
-      <c r="E26" s="8"/>
-      <c r="F26" s="8"/>
-      <c r="G26" s="8"/>
-      <c r="H26" s="9"/>
+      <c r="B26" s="18"/>
+      <c r="C26" s="5"/>
+      <c r="D26" s="6"/>
+      <c r="E26" s="6"/>
+      <c r="F26" s="6"/>
+      <c r="G26" s="6"/>
+      <c r="H26" s="7"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B27" s="3"/>
-      <c r="C27" s="10"/>
-      <c r="D27" s="11"/>
-      <c r="E27" s="11"/>
-      <c r="F27" s="11"/>
-      <c r="G27" s="11"/>
-      <c r="H27" s="12"/>
+      <c r="B27" s="14"/>
+      <c r="C27" s="8"/>
+      <c r="D27" s="9"/>
+      <c r="E27" s="9"/>
+      <c r="F27" s="9"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="10"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B28" s="2"/>
-      <c r="C28" s="7"/>
-      <c r="D28" s="8"/>
-      <c r="E28" s="8"/>
-      <c r="F28" s="8"/>
-      <c r="G28" s="8"/>
-      <c r="H28" s="9"/>
+      <c r="B28" s="18"/>
+      <c r="C28" s="5"/>
+      <c r="D28" s="6"/>
+      <c r="E28" s="6"/>
+      <c r="F28" s="6"/>
+      <c r="G28" s="6"/>
+      <c r="H28" s="7"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B29" s="3"/>
-      <c r="C29" s="10"/>
-      <c r="D29" s="11"/>
-      <c r="E29" s="11"/>
-      <c r="F29" s="11"/>
-      <c r="G29" s="11"/>
-      <c r="H29" s="12"/>
+      <c r="B29" s="14"/>
+      <c r="C29" s="8"/>
+      <c r="D29" s="9"/>
+      <c r="E29" s="9"/>
+      <c r="F29" s="9"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="10"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B30" s="2"/>
-      <c r="C30" s="7"/>
-      <c r="D30" s="8"/>
-      <c r="E30" s="8"/>
-      <c r="F30" s="8"/>
-      <c r="G30" s="8"/>
-      <c r="H30" s="9"/>
+      <c r="B30" s="18"/>
+      <c r="C30" s="5"/>
+      <c r="D30" s="6"/>
+      <c r="E30" s="6"/>
+      <c r="F30" s="6"/>
+      <c r="G30" s="6"/>
+      <c r="H30" s="7"/>
     </row>
     <row r="31" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B31" s="3"/>
-      <c r="C31" s="10"/>
-      <c r="D31" s="11"/>
-      <c r="E31" s="11"/>
-      <c r="F31" s="11"/>
-      <c r="G31" s="11"/>
-      <c r="H31" s="12"/>
+      <c r="B31" s="14"/>
+      <c r="C31" s="8"/>
+      <c r="D31" s="9"/>
+      <c r="E31" s="9"/>
+      <c r="F31" s="9"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="10"/>
     </row>
     <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="2"/>
-      <c r="C32" s="7"/>
-      <c r="D32" s="8"/>
-      <c r="E32" s="8"/>
-      <c r="F32" s="8"/>
-      <c r="G32" s="8"/>
-      <c r="H32" s="9"/>
+      <c r="B32" s="18"/>
+      <c r="C32" s="5"/>
+      <c r="D32" s="6"/>
+      <c r="E32" s="6"/>
+      <c r="F32" s="6"/>
+      <c r="G32" s="6"/>
+      <c r="H32" s="7"/>
     </row>
     <row r="33" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B33" s="3"/>
-      <c r="C33" s="10"/>
-      <c r="D33" s="11"/>
-      <c r="E33" s="11"/>
-      <c r="F33" s="11"/>
-      <c r="G33" s="11"/>
-      <c r="H33" s="12"/>
+      <c r="B33" s="14"/>
+      <c r="C33" s="8"/>
+      <c r="D33" s="9"/>
+      <c r="E33" s="9"/>
+      <c r="F33" s="9"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="10"/>
     </row>
   </sheetData>
-  <mergeCells count="28">
-    <mergeCell ref="C3:H3"/>
-    <mergeCell ref="C22:H23"/>
-    <mergeCell ref="C26:H27"/>
-    <mergeCell ref="C28:H29"/>
-    <mergeCell ref="C30:H31"/>
+  <mergeCells count="27">
+    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="B20:B23"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B26:B27"/>
+    <mergeCell ref="B28:B29"/>
     <mergeCell ref="B10:B15"/>
     <mergeCell ref="C32:H33"/>
     <mergeCell ref="C24:H25"/>
@@ -957,13 +932,11 @@
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="B8:B9"/>
     <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B20:B21"/>
-    <mergeCell ref="B22:B23"/>
-    <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B26:B27"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B16:B19"/>
+    <mergeCell ref="C3:H3"/>
+    <mergeCell ref="C22:H23"/>
+    <mergeCell ref="C26:H27"/>
+    <mergeCell ref="C28:H29"/>
+    <mergeCell ref="C30:H31"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>

</xml_diff>